<commit_message>
added 50XC speed test results
</commit_message>
<xml_diff>
--- a/chansim/Examples/speed-tests/Speed-test-results.xlsx
+++ b/chansim/Examples/speed-tests/Speed-test-results.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="20">
   <si>
     <t xml:space="preserve">Description</t>
   </si>
@@ -89,11 +89,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -113,11 +114,6 @@
     <font>
       <b val="true"/>
       <u val="single"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -175,7 +171,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -199,18 +195,18 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.4795918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="18.0612244897959"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.4744897959184"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="38.4795918367347"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.3979591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="17.6836734693878"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.9336734693878"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.9030612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -377,6 +373,21 @@
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>18</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>2631</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>10000</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>15</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>19</v>

</xml_diff>